<commit_message>
Full dataset & dara corr.
</commit_message>
<xml_diff>
--- a/migforecasting/cities10/0/d6.xlsx
+++ b/migforecasting/cities10/0/d6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities10\0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="329">
   <si>
     <t>Волгоград</t>
   </si>
@@ -1399,7 +1399,7 @@
   <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,11 +1725,11 @@
       <c r="F17" t="s">
         <v>56</v>
       </c>
-      <c r="G17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" t="s">
-        <v>57</v>
+      <c r="G17">
+        <v>1037</v>
+      </c>
+      <c r="H17">
+        <v>689</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>